<commit_message>
major improvements to preventing back-to-back scheduling issues
</commit_message>
<xml_diff>
--- a/data/TT/Division-2020.xlsx
+++ b/data/TT/Division-2020.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\DjangoLeagueScheduler\data\TT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089F8602-36A4-457E-A11F-B82E5D0135A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403DB182-021F-484B-BE3E-E0523A76721B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablib Dataset" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -37,16 +47,16 @@
     <t>league</t>
   </si>
   <si>
-    <t>East</t>
-  </si>
-  <si>
-    <t>West</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>W</t>
+    <t>NationalLeague</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>AmericanLeague</t>
+  </si>
+  <si>
+    <t>AL</t>
   </si>
 </sst>
 </file>
@@ -398,7 +408,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,7 +441,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -442,7 +452,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -459,7 +469,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -470,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
@@ -487,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -498,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -515,7 +525,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -526,7 +536,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
@@ -543,7 +553,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10">
         <v>5</v>
@@ -554,7 +564,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -571,7 +581,7 @@
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12">
         <v>6</v>
@@ -582,7 +592,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>

</xml_diff>